<commit_message>
Admin Preview File dan add link di template excel
</commit_message>
<xml_diff>
--- a/public/articles/TemplateSLR.xlsx
+++ b/public/articles/TemplateSLR.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Kuliah\Tugas Akhir\Project Tugas Akhir\assets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Kuliah\Tugas Akhir\Project Tugas Akhir\SLR_APP\public\articles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0080EA18-1DD7-4DDD-B0AF-56E0D77F7375}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1371A98B-18AA-418B-8A54-4AE9BCBC0509}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>No</t>
   </si>
@@ -94,6 +94,9 @@
   </si>
   <si>
     <t>Nation_First Author</t>
+  </si>
+  <si>
+    <t>Link Articles</t>
   </si>
 </sst>
 </file>
@@ -384,13 +387,13 @@
   <sheetPr>
     <tabColor rgb="FF00B050"/>
   </sheetPr>
-  <dimension ref="A1:V726"/>
+  <dimension ref="A1:W726"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="N2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C3" sqref="C3"/>
+      <selection pane="bottomRight" activeCell="T11" sqref="T11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -417,7 +420,7 @@
     <col min="22" max="22" width="13.25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" ht="49.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:23" ht="49.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -484,8 +487,11 @@
       <c r="V1" s="2" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="2" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="W1" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="5"/>
       <c r="B2" s="3"/>
       <c r="C2" s="4"/>
@@ -509,7 +515,7 @@
       <c r="U2" s="4"/>
       <c r="V2" s="4"/>
     </row>
-    <row r="3" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="5"/>
       <c r="B3" s="3"/>
       <c r="C3" s="4"/>
@@ -533,7 +539,7 @@
       <c r="U3" s="4"/>
       <c r="V3" s="4"/>
     </row>
-    <row r="4" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="5"/>
       <c r="B4" s="3"/>
       <c r="C4" s="4"/>
@@ -557,7 +563,7 @@
       <c r="U4" s="4"/>
       <c r="V4" s="4"/>
     </row>
-    <row r="5" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="5"/>
       <c r="B5" s="3"/>
       <c r="C5" s="4"/>
@@ -581,7 +587,7 @@
       <c r="U5" s="4"/>
       <c r="V5" s="4"/>
     </row>
-    <row r="6" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="5"/>
       <c r="B6" s="3"/>
       <c r="C6" s="4"/>
@@ -605,7 +611,7 @@
       <c r="U6" s="4"/>
       <c r="V6" s="4"/>
     </row>
-    <row r="7" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="5"/>
       <c r="B7" s="3"/>
       <c r="C7" s="4"/>
@@ -629,7 +635,7 @@
       <c r="U7" s="4"/>
       <c r="V7" s="4"/>
     </row>
-    <row r="8" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="5"/>
       <c r="B8" s="3"/>
       <c r="C8" s="4"/>
@@ -653,7 +659,7 @@
       <c r="U8" s="4"/>
       <c r="V8" s="4"/>
     </row>
-    <row r="9" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="5"/>
       <c r="B9" s="3"/>
       <c r="C9" s="4"/>
@@ -677,7 +683,7 @@
       <c r="U9" s="4"/>
       <c r="V9" s="4"/>
     </row>
-    <row r="10" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="5"/>
       <c r="B10" s="3"/>
       <c r="C10" s="4"/>
@@ -701,7 +707,7 @@
       <c r="U10" s="4"/>
       <c r="V10" s="4"/>
     </row>
-    <row r="11" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="5"/>
       <c r="B11" s="3"/>
       <c r="C11" s="4"/>
@@ -725,7 +731,7 @@
       <c r="U11" s="4"/>
       <c r="V11" s="4"/>
     </row>
-    <row r="12" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="5"/>
       <c r="B12" s="3"/>
       <c r="C12" s="4"/>
@@ -749,7 +755,7 @@
       <c r="U12" s="4"/>
       <c r="V12" s="4"/>
     </row>
-    <row r="13" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="5"/>
       <c r="B13" s="3"/>
       <c r="C13" s="4"/>
@@ -773,7 +779,7 @@
       <c r="U13" s="4"/>
       <c r="V13" s="4"/>
     </row>
-    <row r="14" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="5"/>
       <c r="B14" s="3"/>
       <c r="C14" s="4"/>
@@ -797,7 +803,7 @@
       <c r="U14" s="4"/>
       <c r="V14" s="4"/>
     </row>
-    <row r="15" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="5"/>
       <c r="B15" s="3"/>
       <c r="C15" s="4"/>
@@ -821,7 +827,7 @@
       <c r="U15" s="4"/>
       <c r="V15" s="4"/>
     </row>
-    <row r="16" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="5"/>
       <c r="B16" s="3"/>
       <c r="C16" s="4"/>

</xml_diff>